<commit_message>
MS: added unit tests for additional conversion arguments; additional notes for conversion cases
git-svn-id: svn://ms72.weblink.ch/mirai/XLConnect-R@189 ccc6e944-403e-a54a-b5f3-c2babcd103ea
</commit_message>
<xml_diff>
--- a/inst/unitTests/resources/testWorkbookReadNamedRegion.xlsx
+++ b/inst/unitTests/resources/testWorkbookReadNamedRegion.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="20115" windowHeight="8250"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="20115" windowHeight="8250" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Conversion" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="Conversion">Conversion!$B$6:$E$11</definedName>
     <definedName name="Test">Test!$D$5:$G$10</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -17,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>NumericColumn</t>
   </si>
@@ -35,6 +37,48 @@
   </si>
   <si>
     <t>World</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>BBB</t>
+  </si>
+  <si>
+    <t>CCC</t>
+  </si>
+  <si>
+    <t>DDD</t>
+  </si>
+  <si>
+    <t>-14.65</t>
+  </si>
+  <si>
+    <t>not-a-number</t>
+  </si>
+  <si>
+    <t>11.7</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>not-a-boolean</t>
+  </si>
+  <si>
+    <t>06.02.2012 16:15:23</t>
+  </si>
+  <si>
+    <t>not-a-date</t>
+  </si>
+  <si>
+    <t>11.01.1984 12:00:00</t>
   </si>
 </sst>
 </file>
@@ -42,7 +86,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -87,11 +131,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -388,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D5:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -463,4 +510,100 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B6:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:5">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>30692.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>42.24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10">
+        <v>780.9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="C11" s="4">
+        <v>30692.5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="6">
+        <v>357.67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MS: prep for 0.2-0 release; fixing issues with lazy evaluation and S4 generics; readWorksheet returns _named_ list if multiple worksheets are queried by name; introducing check.names parameter for readNamedRegion and readWorksheet
git-svn-id: svn://ms72.weblink.ch/mirai/XLConnect-R@221 ccc6e944-403e-a54a-b5f3-c2babcd103ea
</commit_message>
<xml_diff>
--- a/inst/unitTests/resources/testWorkbookReadNamedRegion.xlsx
+++ b/inst/unitTests/resources/testWorkbookReadNamedRegion.xlsx
@@ -4,22 +4,27 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="20115" windowHeight="8250" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="20115" windowHeight="8250" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
     <sheet name="Conversion" sheetId="2" r:id="rId2"/>
+    <sheet name="Multiple" sheetId="3" r:id="rId3"/>
+    <sheet name="VariableNames" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="AAA">Multiple!$C$6:$E$9</definedName>
+    <definedName name="BBB">Multiple!$I$10:$K$13</definedName>
     <definedName name="Conversion">Conversion!$B$6:$E$11</definedName>
     <definedName name="Test">Test!$D$5:$G$10</definedName>
+    <definedName name="VariableNames">VariableNames!$D$5:$E$9</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>NumericColumn</t>
   </si>
@@ -79,6 +84,48 @@
   </si>
   <si>
     <t>11.01.1984 12:00:00</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>With whitespace</t>
+  </si>
+  <si>
+    <t>And some other funky characters: _=?^~!$@#%§</t>
   </si>
 </sst>
 </file>
@@ -436,7 +483,7 @@
   <dimension ref="D5:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:G10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -516,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B6:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -606,4 +653,166 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C6:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="6" spans="3:11">
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11">
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11">
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11">
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11">
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="D5:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:5">
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5">
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5">
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>